<commit_message>
cleanup figures code, edit the colors in sineplots and western blot figures
</commit_message>
<xml_diff>
--- a/Revisions/Supplementary_Files/Supplementary_File_1/excel files/Supplementary_File_1_Table_1_Gsp1_partner_annotation.xlsx
+++ b/Revisions/Supplementary_Files/Supplementary_File_1/excel files/Supplementary_File_1_Table_1_Gsp1_partner_annotation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tperica/Box Sync/kortemmelab/home/tina/Gsp1_manuscript/Revisions/Supplementary_Files/Supplementary_File_1/excel files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D32042-F447-5A4C-8107-B8329614B5F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DF5356-9EF5-5D48-80BD-DAF6134E7F8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="16240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1032,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScale="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1063,7 +1063,7 @@
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
     </row>
-    <row r="2" spans="1:9" ht="59" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="10" t="s">
         <v>58</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -1584,6 +1584,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;L&amp;"Times New Roman,Bold"&amp;14Supplementary Tables </oddHeader>
+  </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>